<commit_message>
added the invest to the ULP investigator reports
</commit_message>
<xml_diff>
--- a/SMDSDocuments.xlsx
+++ b/SMDSDocuments.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="720" yWindow="915" windowWidth="23235" windowHeight="10455"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6706" uniqueCount="1129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6706" uniqueCount="1130">
   <si>
     <t>ULP</t>
   </si>
@@ -3407,12 +3407,15 @@
   <si>
     <t>Tabled Matter - Supplemental Memo.docx</t>
   </si>
+  <si>
+    <t>Invest</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3483,6 +3486,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -3561,6 +3569,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -3595,6 +3604,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3770,14 +3780,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O479"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="M77" sqref="M77"/>
+    <sheetView tabSelected="1" topLeftCell="A461" workbookViewId="0">
+      <selection activeCell="C483" sqref="C483"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="48.7109375" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="48.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.85546875" customWidth="1"/>
@@ -3800,7 +3810,7 @@
     <col min="20" max="20" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" customHeight="1">
+    <row r="1" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3847,7 +3857,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15" customHeight="1">
+    <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3894,7 +3904,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15" customHeight="1">
+    <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -3941,7 +3951,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="15" customHeight="1">
+    <row r="4" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -3988,7 +3998,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15" customHeight="1">
+    <row r="5" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -4035,7 +4045,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15" customHeight="1">
+    <row r="6" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -4082,7 +4092,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="15" customHeight="1">
+    <row r="7" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -4129,7 +4139,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="15" customHeight="1">
+    <row r="8" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -4176,7 +4186,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="15" customHeight="1">
+    <row r="9" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -4223,7 +4233,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="15" customHeight="1">
+    <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -4270,7 +4280,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="15" customHeight="1">
+    <row r="11" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -4317,7 +4327,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="15" customHeight="1">
+    <row r="12" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -4364,7 +4374,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="15" customHeight="1">
+    <row r="13" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -4411,7 +4421,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="15" customHeight="1">
+    <row r="14" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -4458,7 +4468,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="15" customHeight="1">
+    <row r="15" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -4505,7 +4515,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="15" customHeight="1">
+    <row r="16" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -4552,7 +4562,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="15" customHeight="1">
+    <row r="17" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -4599,7 +4609,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="15" customHeight="1">
+    <row r="18" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -4646,7 +4656,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="15" customHeight="1">
+    <row r="19" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -4693,7 +4703,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="15" customHeight="1">
+    <row r="20" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -4740,7 +4750,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="15" customHeight="1">
+    <row r="21" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -4787,7 +4797,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="15" customHeight="1">
+    <row r="22" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>51</v>
       </c>
@@ -4834,7 +4844,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="15" customHeight="1">
+    <row r="23" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>51</v>
       </c>
@@ -4881,7 +4891,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="15" customHeight="1">
+    <row r="24" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>51</v>
       </c>
@@ -4928,7 +4938,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="15" customHeight="1">
+    <row r="25" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>51</v>
       </c>
@@ -4975,7 +4985,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="15" customHeight="1">
+    <row r="26" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>51</v>
       </c>
@@ -5022,7 +5032,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="15" customHeight="1">
+    <row r="27" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>51</v>
       </c>
@@ -5069,7 +5079,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="15" customHeight="1">
+    <row r="28" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>51</v>
       </c>
@@ -5116,7 +5126,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="15" customHeight="1">
+    <row r="29" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>51</v>
       </c>
@@ -5163,7 +5173,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="15" customHeight="1">
+    <row r="30" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>51</v>
       </c>
@@ -5210,7 +5220,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="15" customHeight="1">
+    <row r="31" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>51</v>
       </c>
@@ -5257,7 +5267,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="15" customHeight="1">
+    <row r="32" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>51</v>
       </c>
@@ -5304,7 +5314,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="15" customHeight="1">
+    <row r="33" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>51</v>
       </c>
@@ -5351,7 +5361,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="15" customHeight="1">
+    <row r="34" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>51</v>
       </c>
@@ -5398,7 +5408,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="15" customHeight="1">
+    <row r="35" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>51</v>
       </c>
@@ -5445,7 +5455,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="15" customHeight="1">
+    <row r="36" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>51</v>
       </c>
@@ -5492,7 +5502,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="15" customHeight="1">
+    <row r="37" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>51</v>
       </c>
@@ -5539,7 +5549,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:15" ht="15" customHeight="1">
+    <row r="38" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>85</v>
       </c>
@@ -5586,7 +5596,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="15" customHeight="1">
+    <row r="39" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>85</v>
       </c>
@@ -5633,7 +5643,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:15" ht="15" customHeight="1">
+    <row r="40" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>85</v>
       </c>
@@ -5680,7 +5690,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:15" ht="15" customHeight="1">
+    <row r="41" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>85</v>
       </c>
@@ -5727,7 +5737,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:15" ht="15" customHeight="1">
+    <row r="42" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>85</v>
       </c>
@@ -5774,7 +5784,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:15" ht="15" customHeight="1">
+    <row r="43" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>85</v>
       </c>
@@ -5821,7 +5831,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:15" ht="15" customHeight="1">
+    <row r="44" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>85</v>
       </c>
@@ -5868,7 +5878,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:15" ht="15" customHeight="1">
+    <row r="45" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>85</v>
       </c>
@@ -5915,7 +5925,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:15" ht="15" customHeight="1">
+    <row r="46" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>85</v>
       </c>
@@ -5962,7 +5972,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:15" ht="15" customHeight="1">
+    <row r="47" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>85</v>
       </c>
@@ -6009,7 +6019,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:15" ht="15" customHeight="1">
+    <row r="48" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>85</v>
       </c>
@@ -6056,7 +6066,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:15" ht="15" customHeight="1">
+    <row r="49" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>85</v>
       </c>
@@ -6103,7 +6113,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:15" ht="15" customHeight="1">
+    <row r="50" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>85</v>
       </c>
@@ -6150,7 +6160,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:15" ht="15" customHeight="1">
+    <row r="51" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>85</v>
       </c>
@@ -6197,7 +6207,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:15" ht="15" customHeight="1">
+    <row r="52" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>85</v>
       </c>
@@ -6244,7 +6254,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:15" ht="15" customHeight="1">
+    <row r="53" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>85</v>
       </c>
@@ -6291,7 +6301,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:15" ht="15" customHeight="1">
+    <row r="54" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>85</v>
       </c>
@@ -6338,7 +6348,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:15" ht="15" customHeight="1">
+    <row r="55" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>85</v>
       </c>
@@ -6385,7 +6395,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:15" ht="15" customHeight="1">
+    <row r="56" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>85</v>
       </c>
@@ -6432,7 +6442,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:15" ht="15" customHeight="1">
+    <row r="57" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>85</v>
       </c>
@@ -6479,7 +6489,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:15" ht="15" customHeight="1">
+    <row r="58" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>85</v>
       </c>
@@ -6526,7 +6536,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:15" ht="15" customHeight="1">
+    <row r="59" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>85</v>
       </c>
@@ -6573,7 +6583,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:15" ht="15" customHeight="1">
+    <row r="60" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>85</v>
       </c>
@@ -6620,7 +6630,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="1:15" ht="15" customHeight="1">
+    <row r="61" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>85</v>
       </c>
@@ -6667,7 +6677,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:15" ht="15" customHeight="1">
+    <row r="62" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>85</v>
       </c>
@@ -6714,7 +6724,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:15" ht="15" customHeight="1">
+    <row r="63" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>135</v>
       </c>
@@ -6761,7 +6771,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:15" ht="15" customHeight="1">
+    <row r="64" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>135</v>
       </c>
@@ -6808,7 +6818,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:15" ht="15" customHeight="1">
+    <row r="65" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>135</v>
       </c>
@@ -6855,7 +6865,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:15" ht="15" customHeight="1">
+    <row r="66" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>135</v>
       </c>
@@ -6902,7 +6912,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:15" ht="15" customHeight="1">
+    <row r="67" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>135</v>
       </c>
@@ -6949,7 +6959,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:15" ht="15" customHeight="1">
+    <row r="68" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>135</v>
       </c>
@@ -6996,7 +7006,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:15" ht="15" customHeight="1">
+    <row r="69" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>135</v>
       </c>
@@ -7043,7 +7053,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:15" ht="15" customHeight="1">
+    <row r="70" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>135</v>
       </c>
@@ -7090,7 +7100,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="1:15" ht="15" customHeight="1">
+    <row r="71" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>135</v>
       </c>
@@ -7137,7 +7147,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:15" ht="15" customHeight="1">
+    <row r="72" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>135</v>
       </c>
@@ -7184,7 +7194,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:15" ht="15" customHeight="1">
+    <row r="73" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>135</v>
       </c>
@@ -7231,7 +7241,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="74" spans="1:15" ht="15" customHeight="1">
+    <row r="74" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>135</v>
       </c>
@@ -7278,7 +7288,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="1:15" ht="15" customHeight="1">
+    <row r="75" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>163</v>
       </c>
@@ -7325,7 +7335,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:15" ht="15" customHeight="1">
+    <row r="76" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>163</v>
       </c>
@@ -7372,7 +7382,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:15" ht="15" customHeight="1">
+    <row r="77" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>163</v>
       </c>
@@ -7419,7 +7429,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="1:15" ht="15" customHeight="1">
+    <row r="78" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>170</v>
       </c>
@@ -7466,7 +7476,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="1:15" ht="15" customHeight="1">
+    <row r="79" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>170</v>
       </c>
@@ -7513,7 +7523,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="80" spans="1:15" ht="15" customHeight="1">
+    <row r="80" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>170</v>
       </c>
@@ -7560,7 +7570,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="81" spans="1:15" ht="15" customHeight="1">
+    <row r="81" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>170</v>
       </c>
@@ -7607,7 +7617,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:15" ht="15" customHeight="1">
+    <row r="82" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>170</v>
       </c>
@@ -7654,7 +7664,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="83" spans="1:15" ht="15" customHeight="1">
+    <row r="83" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>181</v>
       </c>
@@ -7701,7 +7711,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="84" spans="1:15" ht="15" customHeight="1">
+    <row r="84" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>181</v>
       </c>
@@ -7748,7 +7758,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="85" spans="1:15" ht="15" customHeight="1">
+    <row r="85" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>181</v>
       </c>
@@ -7795,7 +7805,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="86" spans="1:15" ht="15" customHeight="1">
+    <row r="86" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>181</v>
       </c>
@@ -7842,7 +7852,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="87" spans="1:15" ht="15" customHeight="1">
+    <row r="87" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>181</v>
       </c>
@@ -7889,7 +7899,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="88" spans="1:15" ht="15" customHeight="1">
+    <row r="88" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>181</v>
       </c>
@@ -7936,7 +7946,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="89" spans="1:15" ht="15" customHeight="1">
+    <row r="89" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>85</v>
       </c>
@@ -7983,7 +7993,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="90" spans="1:15" ht="15" customHeight="1">
+    <row r="90" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>85</v>
       </c>
@@ -8030,7 +8040,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="91" spans="1:15" ht="15" customHeight="1">
+    <row r="91" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>85</v>
       </c>
@@ -8077,7 +8087,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="92" spans="1:15" ht="15" customHeight="1">
+    <row r="92" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>85</v>
       </c>
@@ -8124,7 +8134,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="93" spans="1:15" ht="15" customHeight="1">
+    <row r="93" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>85</v>
       </c>
@@ -8171,7 +8181,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="94" spans="1:15" ht="15" customHeight="1">
+    <row r="94" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>85</v>
       </c>
@@ -8218,7 +8228,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="95" spans="1:15" ht="15" customHeight="1">
+    <row r="95" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>85</v>
       </c>
@@ -8265,7 +8275,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="96" spans="1:15" ht="15" customHeight="1">
+    <row r="96" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>85</v>
       </c>
@@ -8312,7 +8322,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="97" spans="1:15" ht="15" customHeight="1">
+    <row r="97" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>85</v>
       </c>
@@ -8359,7 +8369,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="98" spans="1:15" ht="15" customHeight="1">
+    <row r="98" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>85</v>
       </c>
@@ -8406,7 +8416,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="99" spans="1:15" ht="15" customHeight="1">
+    <row r="99" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>85</v>
       </c>
@@ -8453,7 +8463,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="100" spans="1:15" ht="15" customHeight="1">
+    <row r="100" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>85</v>
       </c>
@@ -8500,7 +8510,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="101" spans="1:15" ht="15" customHeight="1">
+    <row r="101" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>85</v>
       </c>
@@ -8547,7 +8557,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="102" spans="1:15" ht="15" customHeight="1">
+    <row r="102" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>85</v>
       </c>
@@ -8594,7 +8604,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="103" spans="1:15" ht="15" customHeight="1">
+    <row r="103" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>85</v>
       </c>
@@ -8641,7 +8651,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="104" spans="1:15" ht="15" customHeight="1">
+    <row r="104" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>85</v>
       </c>
@@ -8688,7 +8698,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="105" spans="1:15" ht="15" customHeight="1">
+    <row r="105" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>85</v>
       </c>
@@ -8735,7 +8745,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="106" spans="1:15" ht="15" customHeight="1">
+    <row r="106" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>85</v>
       </c>
@@ -8782,7 +8792,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="107" spans="1:15" ht="15" customHeight="1">
+    <row r="107" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>85</v>
       </c>
@@ -8829,7 +8839,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="108" spans="1:15" ht="15" customHeight="1">
+    <row r="108" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>85</v>
       </c>
@@ -8876,7 +8886,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="109" spans="1:15" ht="15" customHeight="1">
+    <row r="109" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>85</v>
       </c>
@@ -8923,7 +8933,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="110" spans="1:15" ht="15" customHeight="1">
+    <row r="110" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>85</v>
       </c>
@@ -8970,7 +8980,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="111" spans="1:15" ht="15" customHeight="1">
+    <row r="111" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>85</v>
       </c>
@@ -9017,7 +9027,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="112" spans="1:15" ht="15" customHeight="1">
+    <row r="112" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>85</v>
       </c>
@@ -9064,7 +9074,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="113" spans="1:15" ht="15" customHeight="1">
+    <row r="113" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>85</v>
       </c>
@@ -9111,7 +9121,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="114" spans="1:15" ht="15" customHeight="1">
+    <row r="114" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>85</v>
       </c>
@@ -9158,7 +9168,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="115" spans="1:15" ht="15" customHeight="1">
+    <row r="115" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>85</v>
       </c>
@@ -9205,7 +9215,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="116" spans="1:15" ht="15" customHeight="1">
+    <row r="116" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>85</v>
       </c>
@@ -9252,7 +9262,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="117" spans="1:15" ht="15" customHeight="1">
+    <row r="117" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>85</v>
       </c>
@@ -9299,7 +9309,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="118" spans="1:15" ht="15" customHeight="1">
+    <row r="118" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>85</v>
       </c>
@@ -9346,7 +9356,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="119" spans="1:15" ht="15" customHeight="1">
+    <row r="119" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>135</v>
       </c>
@@ -9393,7 +9403,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="120" spans="1:15" ht="15" customHeight="1">
+    <row r="120" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>135</v>
       </c>
@@ -9440,7 +9450,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="121" spans="1:15" ht="15" customHeight="1">
+    <row r="121" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>135</v>
       </c>
@@ -9487,7 +9497,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="122" spans="1:15" ht="15" customHeight="1">
+    <row r="122" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>135</v>
       </c>
@@ -9534,7 +9544,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="123" spans="1:15" ht="15" customHeight="1">
+    <row r="123" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>135</v>
       </c>
@@ -9581,7 +9591,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="124" spans="1:15" ht="15" customHeight="1">
+    <row r="124" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>135</v>
       </c>
@@ -9628,7 +9638,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="125" spans="1:15" ht="15" customHeight="1">
+    <row r="125" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>51</v>
       </c>
@@ -9675,7 +9685,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="126" spans="1:15" ht="15" customHeight="1">
+    <row r="126" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>51</v>
       </c>
@@ -9722,7 +9732,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="127" spans="1:15" ht="15" customHeight="1">
+    <row r="127" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>51</v>
       </c>
@@ -9769,7 +9779,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="128" spans="1:15" ht="15" customHeight="1">
+    <row r="128" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>51</v>
       </c>
@@ -9816,7 +9826,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="129" spans="1:15" ht="15" customHeight="1">
+    <row r="129" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>51</v>
       </c>
@@ -9863,7 +9873,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="130" spans="1:15" ht="15" customHeight="1">
+    <row r="130" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>51</v>
       </c>
@@ -9910,7 +9920,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="131" spans="1:15" ht="15" customHeight="1">
+    <row r="131" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>51</v>
       </c>
@@ -9957,7 +9967,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="132" spans="1:15" ht="15" customHeight="1">
+    <row r="132" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>51</v>
       </c>
@@ -10004,7 +10014,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="133" spans="1:15" ht="15" customHeight="1">
+    <row r="133" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>51</v>
       </c>
@@ -10051,7 +10061,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="134" spans="1:15" ht="15" customHeight="1">
+    <row r="134" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>51</v>
       </c>
@@ -10098,7 +10108,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="135" spans="1:15" ht="15" customHeight="1">
+    <row r="135" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>51</v>
       </c>
@@ -10145,7 +10155,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="136" spans="1:15" ht="15" customHeight="1">
+    <row r="136" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>51</v>
       </c>
@@ -10192,7 +10202,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="137" spans="1:15" ht="15" customHeight="1">
+    <row r="137" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>51</v>
       </c>
@@ -10239,7 +10249,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="138" spans="1:15" ht="15" customHeight="1">
+    <row r="138" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>51</v>
       </c>
@@ -10286,7 +10296,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="139" spans="1:15" ht="15" customHeight="1">
+    <row r="139" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>51</v>
       </c>
@@ -10333,7 +10343,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="140" spans="1:15" ht="15" customHeight="1">
+    <row r="140" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>51</v>
       </c>
@@ -10380,7 +10390,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="141" spans="1:15" ht="15" customHeight="1">
+    <row r="141" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>51</v>
       </c>
@@ -10427,7 +10437,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="142" spans="1:15" ht="15" customHeight="1">
+    <row r="142" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>51</v>
       </c>
@@ -10474,7 +10484,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="143" spans="1:15" ht="15" customHeight="1">
+    <row r="143" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>51</v>
       </c>
@@ -10521,7 +10531,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="144" spans="1:15" ht="15" customHeight="1">
+    <row r="144" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>51</v>
       </c>
@@ -10568,7 +10578,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="145" spans="1:15" ht="15" customHeight="1">
+    <row r="145" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>51</v>
       </c>
@@ -10615,7 +10625,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="146" spans="1:15" ht="15" customHeight="1">
+    <row r="146" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>51</v>
       </c>
@@ -10662,7 +10672,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="147" spans="1:15" ht="15" customHeight="1">
+    <row r="147" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>51</v>
       </c>
@@ -10709,7 +10719,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="148" spans="1:15" ht="15" customHeight="1">
+    <row r="148" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>51</v>
       </c>
@@ -10756,7 +10766,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="149" spans="1:15" ht="15" customHeight="1">
+    <row r="149" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>51</v>
       </c>
@@ -10803,7 +10813,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="150" spans="1:15" ht="15" customHeight="1">
+    <row r="150" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>51</v>
       </c>
@@ -10850,7 +10860,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="151" spans="1:15" ht="15" customHeight="1">
+    <row r="151" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>51</v>
       </c>
@@ -10897,7 +10907,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="152" spans="1:15" ht="15" customHeight="1">
+    <row r="152" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>51</v>
       </c>
@@ -10944,7 +10954,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="153" spans="1:15" ht="15" customHeight="1">
+    <row r="153" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>51</v>
       </c>
@@ -10991,7 +11001,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="154" spans="1:15" ht="15" customHeight="1">
+    <row r="154" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>51</v>
       </c>
@@ -11038,7 +11048,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="155" spans="1:15" ht="15" customHeight="1">
+    <row r="155" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>51</v>
       </c>
@@ -11085,7 +11095,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="156" spans="1:15" ht="15" customHeight="1">
+    <row r="156" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>51</v>
       </c>
@@ -11132,7 +11142,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="157" spans="1:15" ht="15" customHeight="1">
+    <row r="157" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>51</v>
       </c>
@@ -11179,7 +11189,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="158" spans="1:15" ht="15" customHeight="1">
+    <row r="158" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>51</v>
       </c>
@@ -11226,7 +11236,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="159" spans="1:15" ht="15" customHeight="1">
+    <row r="159" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>51</v>
       </c>
@@ -11273,7 +11283,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="160" spans="1:15" ht="15" customHeight="1">
+    <row r="160" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>51</v>
       </c>
@@ -11320,7 +11330,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="161" spans="1:15" ht="15" customHeight="1">
+    <row r="161" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>51</v>
       </c>
@@ -11367,7 +11377,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="162" spans="1:15" ht="15" customHeight="1">
+    <row r="162" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>51</v>
       </c>
@@ -11414,7 +11424,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="163" spans="1:15" ht="15" customHeight="1">
+    <row r="163" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>51</v>
       </c>
@@ -11461,7 +11471,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="164" spans="1:15" ht="15" customHeight="1">
+    <row r="164" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>51</v>
       </c>
@@ -11508,7 +11518,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="165" spans="1:15" ht="15" customHeight="1">
+    <row r="165" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>51</v>
       </c>
@@ -11555,7 +11565,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="166" spans="1:15" ht="15" customHeight="1">
+    <row r="166" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>51</v>
       </c>
@@ -11602,7 +11612,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="167" spans="1:15" ht="15" customHeight="1">
+    <row r="167" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>51</v>
       </c>
@@ -11649,7 +11659,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="168" spans="1:15" ht="15" customHeight="1">
+    <row r="168" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>51</v>
       </c>
@@ -11696,7 +11706,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="169" spans="1:15" ht="15" customHeight="1">
+    <row r="169" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>51</v>
       </c>
@@ -11743,7 +11753,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="170" spans="1:15" ht="15" customHeight="1">
+    <row r="170" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>51</v>
       </c>
@@ -11790,7 +11800,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="171" spans="1:15" ht="15" customHeight="1">
+    <row r="171" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>51</v>
       </c>
@@ -11837,7 +11847,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="172" spans="1:15" ht="15" customHeight="1">
+    <row r="172" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
         <v>51</v>
       </c>
@@ -11884,7 +11894,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="173" spans="1:15" ht="15" customHeight="1">
+    <row r="173" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
         <v>51</v>
       </c>
@@ -11931,7 +11941,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="174" spans="1:15" ht="15" customHeight="1">
+    <row r="174" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>51</v>
       </c>
@@ -11978,7 +11988,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="175" spans="1:15" ht="15" customHeight="1">
+    <row r="175" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
         <v>51</v>
       </c>
@@ -12025,7 +12035,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="176" spans="1:15" ht="15" customHeight="1">
+    <row r="176" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
         <v>51</v>
       </c>
@@ -12072,7 +12082,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="177" spans="1:15" ht="15" customHeight="1">
+    <row r="177" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
         <v>51</v>
       </c>
@@ -12119,7 +12129,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="178" spans="1:15" ht="15" customHeight="1">
+    <row r="178" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
         <v>51</v>
       </c>
@@ -12166,7 +12176,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="179" spans="1:15" ht="15" customHeight="1">
+    <row r="179" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
         <v>51</v>
       </c>
@@ -12213,7 +12223,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="180" spans="1:15" ht="15" customHeight="1">
+    <row r="180" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
         <v>51</v>
       </c>
@@ -12260,7 +12270,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="181" spans="1:15" ht="15" customHeight="1">
+    <row r="181" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
         <v>51</v>
       </c>
@@ -12307,7 +12317,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="182" spans="1:15" ht="15" customHeight="1">
+    <row r="182" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
         <v>51</v>
       </c>
@@ -12354,7 +12364,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="183" spans="1:15" ht="15" customHeight="1">
+    <row r="183" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
         <v>51</v>
       </c>
@@ -12401,7 +12411,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="184" spans="1:15" ht="15" customHeight="1">
+    <row r="184" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
         <v>51</v>
       </c>
@@ -12448,7 +12458,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="185" spans="1:15" ht="15" customHeight="1">
+    <row r="185" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
         <v>51</v>
       </c>
@@ -12495,7 +12505,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="186" spans="1:15" ht="15" customHeight="1">
+    <row r="186" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
         <v>51</v>
       </c>
@@ -12542,7 +12552,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="187" spans="1:15" ht="15" customHeight="1">
+    <row r="187" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
         <v>51</v>
       </c>
@@ -12589,7 +12599,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="188" spans="1:15" ht="15" customHeight="1">
+    <row r="188" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
         <v>51</v>
       </c>
@@ -12636,7 +12646,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="189" spans="1:15" ht="15" customHeight="1">
+    <row r="189" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
         <v>51</v>
       </c>
@@ -12683,7 +12693,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="190" spans="1:15" ht="15" customHeight="1">
+    <row r="190" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
         <v>51</v>
       </c>
@@ -12730,7 +12740,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="191" spans="1:15" ht="15" customHeight="1">
+    <row r="191" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="4" t="s">
         <v>51</v>
       </c>
@@ -12777,7 +12787,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="192" spans="1:15" ht="15" customHeight="1">
+    <row r="192" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
         <v>51</v>
       </c>
@@ -12824,7 +12834,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="193" spans="1:15" ht="15" customHeight="1">
+    <row r="193" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
         <v>51</v>
       </c>
@@ -12871,7 +12881,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="194" spans="1:15" ht="15" customHeight="1">
+    <row r="194" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
         <v>51</v>
       </c>
@@ -12918,7 +12928,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="195" spans="1:15" ht="15" customHeight="1">
+    <row r="195" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
         <v>51</v>
       </c>
@@ -12965,7 +12975,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="196" spans="1:15" ht="15" customHeight="1">
+    <row r="196" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
         <v>51</v>
       </c>
@@ -13012,7 +13022,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="197" spans="1:15" ht="15" customHeight="1">
+    <row r="197" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
         <v>51</v>
       </c>
@@ -13059,7 +13069,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="198" spans="1:15" ht="15" customHeight="1">
+    <row r="198" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
         <v>51</v>
       </c>
@@ -13106,7 +13116,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="199" spans="1:15" ht="15" customHeight="1">
+    <row r="199" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
         <v>51</v>
       </c>
@@ -13153,7 +13163,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="200" spans="1:15" ht="15" customHeight="1">
+    <row r="200" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
         <v>51</v>
       </c>
@@ -13200,7 +13210,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="201" spans="1:15" ht="15" customHeight="1">
+    <row r="201" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
         <v>51</v>
       </c>
@@ -13247,7 +13257,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="202" spans="1:15" ht="15" customHeight="1">
+    <row r="202" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
         <v>51</v>
       </c>
@@ -13294,7 +13304,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="203" spans="1:15" ht="15" customHeight="1">
+    <row r="203" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
         <v>51</v>
       </c>
@@ -13341,7 +13351,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="204" spans="1:15" ht="15" customHeight="1">
+    <row r="204" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
         <v>51</v>
       </c>
@@ -13388,7 +13398,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="205" spans="1:15" ht="15" customHeight="1">
+    <row r="205" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
         <v>51</v>
       </c>
@@ -13435,7 +13445,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="206" spans="1:15" ht="15" customHeight="1">
+    <row r="206" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
         <v>51</v>
       </c>
@@ -13482,7 +13492,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="207" spans="1:15" ht="15" customHeight="1">
+    <row r="207" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
         <v>51</v>
       </c>
@@ -13529,7 +13539,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="208" spans="1:15" ht="15" customHeight="1">
+    <row r="208" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
         <v>51</v>
       </c>
@@ -13576,7 +13586,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="209" spans="1:15" ht="15" customHeight="1">
+    <row r="209" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
         <v>51</v>
       </c>
@@ -13623,7 +13633,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="210" spans="1:15" ht="15" customHeight="1">
+    <row r="210" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
         <v>51</v>
       </c>
@@ -13670,7 +13680,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="211" spans="1:15" ht="15" customHeight="1">
+    <row r="211" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
         <v>51</v>
       </c>
@@ -13717,7 +13727,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="212" spans="1:15" ht="15" customHeight="1">
+    <row r="212" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
         <v>51</v>
       </c>
@@ -13764,7 +13774,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="213" spans="1:15" ht="15" customHeight="1">
+    <row r="213" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
         <v>51</v>
       </c>
@@ -13811,7 +13821,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="214" spans="1:15" ht="15" customHeight="1">
+    <row r="214" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
         <v>51</v>
       </c>
@@ -13858,7 +13868,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="215" spans="1:15" ht="15" customHeight="1">
+    <row r="215" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
         <v>51</v>
       </c>
@@ -13905,7 +13915,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="216" spans="1:15" ht="15" customHeight="1">
+    <row r="216" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
         <v>51</v>
       </c>
@@ -13952,7 +13962,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="217" spans="1:15" ht="15" customHeight="1">
+    <row r="217" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
         <v>51</v>
       </c>
@@ -13999,7 +14009,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="218" spans="1:15" ht="15" customHeight="1">
+    <row r="218" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
         <v>51</v>
       </c>
@@ -14046,7 +14056,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="219" spans="1:15" ht="15" customHeight="1">
+    <row r="219" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
         <v>51</v>
       </c>
@@ -14093,7 +14103,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="220" spans="1:15" ht="15" customHeight="1">
+    <row r="220" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
         <v>51</v>
       </c>
@@ -14140,7 +14150,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="221" spans="1:15" ht="15" customHeight="1">
+    <row r="221" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
         <v>51</v>
       </c>
@@ -14187,7 +14197,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="222" spans="1:15" ht="15" customHeight="1">
+    <row r="222" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
         <v>51</v>
       </c>
@@ -14234,7 +14244,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="223" spans="1:15" ht="15" customHeight="1">
+    <row r="223" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
         <v>51</v>
       </c>
@@ -14281,7 +14291,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="224" spans="1:15" ht="15" customHeight="1">
+    <row r="224" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
         <v>51</v>
       </c>
@@ -14328,7 +14338,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="225" spans="1:15" ht="15" customHeight="1">
+    <row r="225" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
         <v>51</v>
       </c>
@@ -14375,7 +14385,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="226" spans="1:15" ht="15" customHeight="1">
+    <row r="226" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
         <v>51</v>
       </c>
@@ -14422,7 +14432,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="227" spans="1:15" ht="15" customHeight="1">
+    <row r="227" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
         <v>51</v>
       </c>
@@ -14469,7 +14479,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="228" spans="1:15" ht="15" customHeight="1">
+    <row r="228" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
         <v>51</v>
       </c>
@@ -14516,7 +14526,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="229" spans="1:15" ht="15" customHeight="1">
+    <row r="229" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
         <v>51</v>
       </c>
@@ -14563,7 +14573,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="230" spans="1:15" ht="15" customHeight="1">
+    <row r="230" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
         <v>51</v>
       </c>
@@ -14610,7 +14620,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="231" spans="1:15" ht="15" customHeight="1">
+    <row r="231" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
         <v>51</v>
       </c>
@@ -14657,7 +14667,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="232" spans="1:15" ht="15" customHeight="1">
+    <row r="232" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
         <v>51</v>
       </c>
@@ -14704,7 +14714,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="233" spans="1:15" ht="15" customHeight="1">
+    <row r="233" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
         <v>51</v>
       </c>
@@ -14751,7 +14761,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="234" spans="1:15" ht="15" customHeight="1">
+    <row r="234" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
         <v>51</v>
       </c>
@@ -14798,7 +14808,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="235" spans="1:15" ht="15" customHeight="1">
+    <row r="235" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A235" s="1" t="s">
         <v>51</v>
       </c>
@@ -14845,7 +14855,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="236" spans="1:15" ht="15" customHeight="1">
+    <row r="236" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
         <v>51</v>
       </c>
@@ -14892,7 +14902,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="237" spans="1:15" ht="15" customHeight="1">
+    <row r="237" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A237" s="1" t="s">
         <v>51</v>
       </c>
@@ -14939,7 +14949,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="238" spans="1:15" ht="15" customHeight="1">
+    <row r="238" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
         <v>51</v>
       </c>
@@ -14986,7 +14996,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="239" spans="1:15" ht="15" customHeight="1">
+    <row r="239" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A239" s="1" t="s">
         <v>51</v>
       </c>
@@ -15033,7 +15043,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="240" spans="1:15" ht="15" customHeight="1">
+    <row r="240" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A240" s="1" t="s">
         <v>51</v>
       </c>
@@ -15080,7 +15090,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="241" spans="1:15" ht="15" customHeight="1">
+    <row r="241" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
         <v>51</v>
       </c>
@@ -15127,7 +15137,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="242" spans="1:15" ht="15" customHeight="1">
+    <row r="242" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
         <v>51</v>
       </c>
@@ -15174,7 +15184,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="243" spans="1:15" ht="15" customHeight="1">
+    <row r="243" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A243" s="1" t="s">
         <v>51</v>
       </c>
@@ -15221,7 +15231,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="244" spans="1:15" ht="15" customHeight="1">
+    <row r="244" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A244" s="1" t="s">
         <v>51</v>
       </c>
@@ -15268,7 +15278,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="245" spans="1:15" ht="15" customHeight="1">
+    <row r="245" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
         <v>51</v>
       </c>
@@ -15315,7 +15325,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="246" spans="1:15" ht="15" customHeight="1">
+    <row r="246" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
         <v>51</v>
       </c>
@@ -15362,7 +15372,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="247" spans="1:15" ht="15" customHeight="1">
+    <row r="247" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
         <v>51</v>
       </c>
@@ -15409,7 +15419,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="248" spans="1:15" ht="15" customHeight="1">
+    <row r="248" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
         <v>51</v>
       </c>
@@ -15456,7 +15466,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="249" spans="1:15" ht="15" customHeight="1">
+    <row r="249" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A249" s="1" t="s">
         <v>51</v>
       </c>
@@ -15503,7 +15513,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="250" spans="1:15" ht="15" customHeight="1">
+    <row r="250" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
         <v>51</v>
       </c>
@@ -15550,7 +15560,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="251" spans="1:15" ht="15" customHeight="1">
+    <row r="251" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
         <v>51</v>
       </c>
@@ -15597,7 +15607,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="252" spans="1:15" ht="15" customHeight="1">
+    <row r="252" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
         <v>51</v>
       </c>
@@ -15644,7 +15654,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="253" spans="1:15" ht="15" customHeight="1">
+    <row r="253" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
         <v>51</v>
       </c>
@@ -15691,7 +15701,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="254" spans="1:15" ht="15" customHeight="1">
+    <row r="254" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A254" s="1" t="s">
         <v>51</v>
       </c>
@@ -15738,7 +15748,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="255" spans="1:15" ht="15" customHeight="1">
+    <row r="255" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A255" s="1" t="s">
         <v>51</v>
       </c>
@@ -15785,7 +15795,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="256" spans="1:15" ht="15" customHeight="1">
+    <row r="256" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A256" s="1" t="s">
         <v>51</v>
       </c>
@@ -15832,7 +15842,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="257" spans="1:15" ht="15" customHeight="1">
+    <row r="257" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A257" s="1" t="s">
         <v>51</v>
       </c>
@@ -15879,7 +15889,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="258" spans="1:15" ht="15" customHeight="1">
+    <row r="258" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A258" s="1" t="s">
         <v>51</v>
       </c>
@@ -15926,7 +15936,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="259" spans="1:15" ht="15" customHeight="1">
+    <row r="259" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A259" s="1" t="s">
         <v>51</v>
       </c>
@@ -15973,7 +15983,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="260" spans="1:15" ht="15" customHeight="1">
+    <row r="260" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
         <v>51</v>
       </c>
@@ -16020,7 +16030,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="261" spans="1:15" ht="15" customHeight="1">
+    <row r="261" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A261" s="1" t="s">
         <v>51</v>
       </c>
@@ -16067,7 +16077,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="262" spans="1:15" ht="15" customHeight="1">
+    <row r="262" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A262" s="1" t="s">
         <v>51</v>
       </c>
@@ -16114,7 +16124,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="263" spans="1:15" ht="15" customHeight="1">
+    <row r="263" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A263" s="1" t="s">
         <v>51</v>
       </c>
@@ -16161,7 +16171,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="264" spans="1:15" ht="15" customHeight="1">
+    <row r="264" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A264" s="1" t="s">
         <v>51</v>
       </c>
@@ -16208,7 +16218,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="265" spans="1:15" ht="15" customHeight="1">
+    <row r="265" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A265" s="1" t="s">
         <v>51</v>
       </c>
@@ -16255,7 +16265,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="266" spans="1:15" ht="15" customHeight="1">
+    <row r="266" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
         <v>51</v>
       </c>
@@ -16302,7 +16312,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="267" spans="1:15" ht="15" customHeight="1">
+    <row r="267" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
         <v>51</v>
       </c>
@@ -16349,7 +16359,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="268" spans="1:15" ht="15" customHeight="1">
+    <row r="268" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
         <v>51</v>
       </c>
@@ -16396,7 +16406,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="269" spans="1:15" ht="15" customHeight="1">
+    <row r="269" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A269" s="1" t="s">
         <v>51</v>
       </c>
@@ -16443,7 +16453,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="270" spans="1:15" ht="15" customHeight="1">
+    <row r="270" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A270" s="1" t="s">
         <v>51</v>
       </c>
@@ -16490,7 +16500,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="271" spans="1:15" ht="15" customHeight="1">
+    <row r="271" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A271" s="1" t="s">
         <v>51</v>
       </c>
@@ -16537,7 +16547,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="272" spans="1:15" ht="15" customHeight="1">
+    <row r="272" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A272" s="1" t="s">
         <v>51</v>
       </c>
@@ -16584,7 +16594,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="273" spans="1:15" ht="15" customHeight="1">
+    <row r="273" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A273" s="1" t="s">
         <v>51</v>
       </c>
@@ -16631,7 +16641,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="274" spans="1:15" ht="15" customHeight="1">
+    <row r="274" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A274" s="1" t="s">
         <v>51</v>
       </c>
@@ -16678,7 +16688,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="275" spans="1:15" ht="15" customHeight="1">
+    <row r="275" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A275" s="1" t="s">
         <v>51</v>
       </c>
@@ -16725,7 +16735,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="276" spans="1:15" ht="15" customHeight="1">
+    <row r="276" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A276" s="1" t="s">
         <v>51</v>
       </c>
@@ -16772,7 +16782,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="277" spans="1:15" ht="15" customHeight="1">
+    <row r="277" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A277" s="1" t="s">
         <v>51</v>
       </c>
@@ -16819,7 +16829,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="278" spans="1:15" ht="15" customHeight="1">
+    <row r="278" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A278" s="1" t="s">
         <v>51</v>
       </c>
@@ -16866,7 +16876,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="279" spans="1:15" ht="15" customHeight="1">
+    <row r="279" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A279" s="1" t="s">
         <v>51</v>
       </c>
@@ -16913,7 +16923,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="280" spans="1:15" ht="15" customHeight="1">
+    <row r="280" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A280" s="1" t="s">
         <v>51</v>
       </c>
@@ -16960,7 +16970,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="281" spans="1:15" ht="15" customHeight="1">
+    <row r="281" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A281" s="1" t="s">
         <v>51</v>
       </c>
@@ -17007,7 +17017,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="282" spans="1:15" ht="15" customHeight="1">
+    <row r="282" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A282" s="1" t="s">
         <v>51</v>
       </c>
@@ -17054,7 +17064,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="283" spans="1:15" ht="15" customHeight="1">
+    <row r="283" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A283" s="1" t="s">
         <v>51</v>
       </c>
@@ -17101,7 +17111,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="284" spans="1:15" ht="15" customHeight="1">
+    <row r="284" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A284" s="1" t="s">
         <v>51</v>
       </c>
@@ -17148,7 +17158,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="285" spans="1:15" ht="15" customHeight="1">
+    <row r="285" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A285" s="1" t="s">
         <v>51</v>
       </c>
@@ -17195,7 +17205,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="286" spans="1:15" ht="15" customHeight="1">
+    <row r="286" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A286" s="1" t="s">
         <v>51</v>
       </c>
@@ -17242,7 +17252,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="287" spans="1:15" ht="15" customHeight="1">
+    <row r="287" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A287" s="1" t="s">
         <v>51</v>
       </c>
@@ -17289,7 +17299,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="288" spans="1:15" ht="15" customHeight="1">
+    <row r="288" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A288" s="1" t="s">
         <v>51</v>
       </c>
@@ -17336,7 +17346,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="289" spans="1:15" ht="15" customHeight="1">
+    <row r="289" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A289" s="1" t="s">
         <v>51</v>
       </c>
@@ -17383,7 +17393,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="290" spans="1:15" ht="15" customHeight="1">
+    <row r="290" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A290" s="1" t="s">
         <v>51</v>
       </c>
@@ -17430,7 +17440,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="291" spans="1:15" ht="15" customHeight="1">
+    <row r="291" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A291" s="1" t="s">
         <v>51</v>
       </c>
@@ -17477,7 +17487,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="292" spans="1:15" ht="15" customHeight="1">
+    <row r="292" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A292" s="1" t="s">
         <v>51</v>
       </c>
@@ -17524,7 +17534,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="293" spans="1:15" ht="15" customHeight="1">
+    <row r="293" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A293" s="1" t="s">
         <v>51</v>
       </c>
@@ -17571,7 +17581,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="294" spans="1:15" ht="15" customHeight="1">
+    <row r="294" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A294" s="1" t="s">
         <v>51</v>
       </c>
@@ -17618,7 +17628,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="295" spans="1:15" ht="15" customHeight="1">
+    <row r="295" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A295" s="1" t="s">
         <v>51</v>
       </c>
@@ -17665,7 +17675,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="296" spans="1:15" ht="15" customHeight="1">
+    <row r="296" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A296" s="1" t="s">
         <v>51</v>
       </c>
@@ -17712,7 +17722,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="297" spans="1:15" ht="15" customHeight="1">
+    <row r="297" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A297" s="1" t="s">
         <v>51</v>
       </c>
@@ -17759,7 +17769,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="298" spans="1:15" ht="15" customHeight="1">
+    <row r="298" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A298" s="1" t="s">
         <v>51</v>
       </c>
@@ -17806,7 +17816,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="299" spans="1:15" ht="15" customHeight="1">
+    <row r="299" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A299" s="1" t="s">
         <v>51</v>
       </c>
@@ -17853,7 +17863,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="300" spans="1:15" ht="15" customHeight="1">
+    <row r="300" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A300" s="1" t="s">
         <v>51</v>
       </c>
@@ -17900,7 +17910,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="301" spans="1:15" ht="15" customHeight="1">
+    <row r="301" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A301" s="1" t="s">
         <v>51</v>
       </c>
@@ -17947,7 +17957,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="302" spans="1:15" ht="15" customHeight="1">
+    <row r="302" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A302" s="1" t="s">
         <v>51</v>
       </c>
@@ -17994,7 +18004,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="303" spans="1:15" ht="15" customHeight="1">
+    <row r="303" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A303" s="1" t="s">
         <v>51</v>
       </c>
@@ -18041,7 +18051,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="304" spans="1:15" ht="15" customHeight="1">
+    <row r="304" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A304" s="1" t="s">
         <v>51</v>
       </c>
@@ -18088,7 +18098,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="305" spans="1:15" ht="15" customHeight="1">
+    <row r="305" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A305" s="1" t="s">
         <v>51</v>
       </c>
@@ -18135,7 +18145,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="306" spans="1:15" ht="15" customHeight="1">
+    <row r="306" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A306" s="1" t="s">
         <v>51</v>
       </c>
@@ -18182,7 +18192,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="307" spans="1:15" ht="15" customHeight="1">
+    <row r="307" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A307" s="1" t="s">
         <v>51</v>
       </c>
@@ -18229,7 +18239,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="308" spans="1:15" ht="15" customHeight="1">
+    <row r="308" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A308" s="1" t="s">
         <v>51</v>
       </c>
@@ -18276,7 +18286,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="309" spans="1:15" ht="15" customHeight="1">
+    <row r="309" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A309" s="1" t="s">
         <v>51</v>
       </c>
@@ -18323,7 +18333,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="310" spans="1:15" ht="15" customHeight="1">
+    <row r="310" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A310" s="1" t="s">
         <v>51</v>
       </c>
@@ -18370,7 +18380,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="311" spans="1:15" ht="15" customHeight="1">
+    <row r="311" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A311" s="1" t="s">
         <v>51</v>
       </c>
@@ -18417,7 +18427,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="312" spans="1:15" ht="15" customHeight="1">
+    <row r="312" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A312" s="1" t="s">
         <v>51</v>
       </c>
@@ -18464,7 +18474,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="313" spans="1:15" ht="15" customHeight="1">
+    <row r="313" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A313" s="1" t="s">
         <v>51</v>
       </c>
@@ -18511,7 +18521,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="314" spans="1:15" ht="15" customHeight="1">
+    <row r="314" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A314" s="1" t="s">
         <v>51</v>
       </c>
@@ -18558,7 +18568,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="315" spans="1:15" ht="15" customHeight="1">
+    <row r="315" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A315" s="1" t="s">
         <v>51</v>
       </c>
@@ -18605,7 +18615,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="316" spans="1:15" ht="15" customHeight="1">
+    <row r="316" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A316" s="1" t="s">
         <v>51</v>
       </c>
@@ -18652,7 +18662,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="317" spans="1:15" ht="15" customHeight="1">
+    <row r="317" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A317" s="1" t="s">
         <v>51</v>
       </c>
@@ -18699,7 +18709,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="318" spans="1:15" ht="15" customHeight="1">
+    <row r="318" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A318" s="1" t="s">
         <v>51</v>
       </c>
@@ -18746,7 +18756,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="319" spans="1:15" ht="15" customHeight="1">
+    <row r="319" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A319" s="1" t="s">
         <v>51</v>
       </c>
@@ -18793,7 +18803,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="320" spans="1:15" ht="15" customHeight="1">
+    <row r="320" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A320" s="1" t="s">
         <v>51</v>
       </c>
@@ -18840,7 +18850,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="321" spans="1:15" ht="15" customHeight="1">
+    <row r="321" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A321" s="1" t="s">
         <v>51</v>
       </c>
@@ -18887,7 +18897,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="322" spans="1:15" ht="15" customHeight="1">
+    <row r="322" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A322" s="1" t="s">
         <v>51</v>
       </c>
@@ -18934,7 +18944,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="323" spans="1:15" ht="15" customHeight="1">
+    <row r="323" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A323" s="1" t="s">
         <v>51</v>
       </c>
@@ -18981,7 +18991,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="324" spans="1:15" ht="15" customHeight="1">
+    <row r="324" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A324" s="1" t="s">
         <v>51</v>
       </c>
@@ -19028,7 +19038,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="325" spans="1:15" ht="15" customHeight="1">
+    <row r="325" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A325" s="1" t="s">
         <v>51</v>
       </c>
@@ -19075,7 +19085,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="326" spans="1:15" ht="15" customHeight="1">
+    <row r="326" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A326" s="1" t="s">
         <v>51</v>
       </c>
@@ -19122,7 +19132,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="327" spans="1:15" ht="15" customHeight="1">
+    <row r="327" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A327" s="1" t="s">
         <v>51</v>
       </c>
@@ -19169,7 +19179,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="328" spans="1:15" ht="15" customHeight="1">
+    <row r="328" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A328" s="1" t="s">
         <v>51</v>
       </c>
@@ -19216,7 +19226,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="329" spans="1:15" ht="15" customHeight="1">
+    <row r="329" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A329" s="1" t="s">
         <v>51</v>
       </c>
@@ -19263,7 +19273,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="330" spans="1:15" ht="15" customHeight="1">
+    <row r="330" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A330" s="1" t="s">
         <v>51</v>
       </c>
@@ -19310,7 +19320,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="331" spans="1:15" ht="15" customHeight="1">
+    <row r="331" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A331" s="1" t="s">
         <v>51</v>
       </c>
@@ -19357,7 +19367,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="332" spans="1:15" ht="15" customHeight="1">
+    <row r="332" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A332" s="1" t="s">
         <v>51</v>
       </c>
@@ -19404,7 +19414,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="333" spans="1:15" ht="15" customHeight="1">
+    <row r="333" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A333" s="1" t="s">
         <v>51</v>
       </c>
@@ -19451,7 +19461,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="334" spans="1:15" ht="15" customHeight="1">
+    <row r="334" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A334" s="1" t="s">
         <v>51</v>
       </c>
@@ -19498,7 +19508,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="335" spans="1:15" ht="15" customHeight="1">
+    <row r="335" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A335" s="1" t="s">
         <v>51</v>
       </c>
@@ -19545,7 +19555,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="336" spans="1:15" ht="15" customHeight="1">
+    <row r="336" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A336" s="1" t="s">
         <v>51</v>
       </c>
@@ -19592,7 +19602,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="337" spans="1:15" ht="15" customHeight="1">
+    <row r="337" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A337" s="1" t="s">
         <v>51</v>
       </c>
@@ -19639,7 +19649,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="338" spans="1:15" ht="15" customHeight="1">
+    <row r="338" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A338" s="1" t="s">
         <v>51</v>
       </c>
@@ -19686,7 +19696,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="339" spans="1:15" ht="15" customHeight="1">
+    <row r="339" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A339" s="1" t="s">
         <v>51</v>
       </c>
@@ -19733,7 +19743,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="340" spans="1:15" ht="15" customHeight="1">
+    <row r="340" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A340" s="1" t="s">
         <v>51</v>
       </c>
@@ -19780,7 +19790,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="341" spans="1:15" ht="15" customHeight="1">
+    <row r="341" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A341" s="1" t="s">
         <v>51</v>
       </c>
@@ -19827,7 +19837,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="342" spans="1:15" ht="15" customHeight="1">
+    <row r="342" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A342" s="1" t="s">
         <v>51</v>
       </c>
@@ -19874,7 +19884,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="343" spans="1:15" ht="15" customHeight="1">
+    <row r="343" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A343" s="1" t="s">
         <v>51</v>
       </c>
@@ -19921,7 +19931,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="344" spans="1:15" ht="15" customHeight="1">
+    <row r="344" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A344" s="1" t="s">
         <v>51</v>
       </c>
@@ -19968,7 +19978,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="345" spans="1:15" ht="15" customHeight="1">
+    <row r="345" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A345" s="1" t="s">
         <v>51</v>
       </c>
@@ -20015,7 +20025,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="346" spans="1:15" ht="15" customHeight="1">
+    <row r="346" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A346" s="1" t="s">
         <v>51</v>
       </c>
@@ -20062,7 +20072,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="347" spans="1:15" ht="15" customHeight="1">
+    <row r="347" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A347" s="1" t="s">
         <v>51</v>
       </c>
@@ -20109,7 +20119,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="348" spans="1:15" ht="15" customHeight="1">
+    <row r="348" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A348" s="1" t="s">
         <v>51</v>
       </c>
@@ -20156,7 +20166,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="349" spans="1:15" ht="15" customHeight="1">
+    <row r="349" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A349" s="1" t="s">
         <v>51</v>
       </c>
@@ -20203,7 +20213,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="350" spans="1:15" ht="15" customHeight="1">
+    <row r="350" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A350" s="1" t="s">
         <v>51</v>
       </c>
@@ -20250,7 +20260,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="351" spans="1:15" ht="15" customHeight="1">
+    <row r="351" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A351" s="1" t="s">
         <v>51</v>
       </c>
@@ -20297,7 +20307,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="352" spans="1:15" ht="15" customHeight="1">
+    <row r="352" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A352" s="1" t="s">
         <v>51</v>
       </c>
@@ -20344,7 +20354,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="353" spans="1:15" ht="15" customHeight="1">
+    <row r="353" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A353" s="1" t="s">
         <v>51</v>
       </c>
@@ -20391,7 +20401,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="354" spans="1:15" ht="15" customHeight="1">
+    <row r="354" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A354" s="1" t="s">
         <v>51</v>
       </c>
@@ -20438,7 +20448,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="355" spans="1:15" ht="15" customHeight="1">
+    <row r="355" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A355" s="1" t="s">
         <v>51</v>
       </c>
@@ -20485,7 +20495,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="356" spans="1:15" ht="15" customHeight="1">
+    <row r="356" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A356" s="1" t="s">
         <v>51</v>
       </c>
@@ -20532,7 +20542,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="357" spans="1:15" ht="15" customHeight="1">
+    <row r="357" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A357" s="1" t="s">
         <v>51</v>
       </c>
@@ -20579,7 +20589,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="358" spans="1:15" ht="15" customHeight="1">
+    <row r="358" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A358" s="1" t="s">
         <v>51</v>
       </c>
@@ -20626,7 +20636,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="359" spans="1:15" ht="15" customHeight="1">
+    <row r="359" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A359" s="1" t="s">
         <v>51</v>
       </c>
@@ -20673,7 +20683,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="360" spans="1:15" ht="15" customHeight="1">
+    <row r="360" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A360" s="1" t="s">
         <v>51</v>
       </c>
@@ -20720,7 +20730,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="361" spans="1:15" ht="15" customHeight="1">
+    <row r="361" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A361" s="1" t="s">
         <v>51</v>
       </c>
@@ -20767,7 +20777,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="362" spans="1:15" ht="15" customHeight="1">
+    <row r="362" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A362" s="1" t="s">
         <v>51</v>
       </c>
@@ -20814,7 +20824,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="363" spans="1:15" ht="15" customHeight="1">
+    <row r="363" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A363" s="1" t="s">
         <v>51</v>
       </c>
@@ -20861,7 +20871,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="364" spans="1:15" ht="15" customHeight="1">
+    <row r="364" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A364" s="1" t="s">
         <v>51</v>
       </c>
@@ -20908,7 +20918,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="365" spans="1:15" ht="15" customHeight="1">
+    <row r="365" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A365" s="1" t="s">
         <v>51</v>
       </c>
@@ -20955,7 +20965,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="366" spans="1:15" ht="15" customHeight="1">
+    <row r="366" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A366" s="1" t="s">
         <v>51</v>
       </c>
@@ -21002,7 +21012,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="367" spans="1:15" ht="15" customHeight="1">
+    <row r="367" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A367" s="1" t="s">
         <v>51</v>
       </c>
@@ -21049,7 +21059,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="368" spans="1:15" ht="15" customHeight="1">
+    <row r="368" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A368" s="1" t="s">
         <v>51</v>
       </c>
@@ -21096,7 +21106,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="369" spans="1:15" ht="15" customHeight="1">
+    <row r="369" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A369" s="1" t="s">
         <v>51</v>
       </c>
@@ -21143,7 +21153,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="370" spans="1:15" ht="15" customHeight="1">
+    <row r="370" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A370" s="1" t="s">
         <v>51</v>
       </c>
@@ -21190,7 +21200,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="371" spans="1:15" ht="15" customHeight="1">
+    <row r="371" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A371" s="1" t="s">
         <v>51</v>
       </c>
@@ -21237,7 +21247,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="372" spans="1:15" ht="15" customHeight="1">
+    <row r="372" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A372" s="1" t="s">
         <v>51</v>
       </c>
@@ -21284,7 +21294,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="373" spans="1:15" ht="15" customHeight="1">
+    <row r="373" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A373" s="1" t="s">
         <v>51</v>
       </c>
@@ -21331,7 +21341,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="374" spans="1:15" ht="15" customHeight="1">
+    <row r="374" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A374" s="1" t="s">
         <v>51</v>
       </c>
@@ -21378,7 +21388,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="375" spans="1:15" ht="15" customHeight="1">
+    <row r="375" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A375" s="1" t="s">
         <v>51</v>
       </c>
@@ -21425,7 +21435,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="376" spans="1:15" ht="15" customHeight="1">
+    <row r="376" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A376" s="1" t="s">
         <v>51</v>
       </c>
@@ -21472,7 +21482,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="377" spans="1:15" ht="15" customHeight="1">
+    <row r="377" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A377" s="1" t="s">
         <v>51</v>
       </c>
@@ -21519,7 +21529,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="378" spans="1:15" ht="15" customHeight="1">
+    <row r="378" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A378" s="1" t="s">
         <v>51</v>
       </c>
@@ -21566,7 +21576,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="379" spans="1:15" ht="15" customHeight="1">
+    <row r="379" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A379" s="1" t="s">
         <v>51</v>
       </c>
@@ -21613,7 +21623,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="380" spans="1:15" ht="15" customHeight="1">
+    <row r="380" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A380" s="1" t="s">
         <v>51</v>
       </c>
@@ -21660,7 +21670,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="381" spans="1:15" ht="15" customHeight="1">
+    <row r="381" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A381" s="1" t="s">
         <v>51</v>
       </c>
@@ -21707,7 +21717,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="382" spans="1:15" ht="15" customHeight="1">
+    <row r="382" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A382" s="1" t="s">
         <v>51</v>
       </c>
@@ -21754,7 +21764,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="383" spans="1:15" ht="15" customHeight="1">
+    <row r="383" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A383" s="1" t="s">
         <v>51</v>
       </c>
@@ -21801,7 +21811,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="384" spans="1:15" ht="15" customHeight="1">
+    <row r="384" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A384" s="1" t="s">
         <v>51</v>
       </c>
@@ -21848,7 +21858,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="385" spans="1:15" ht="15" customHeight="1">
+    <row r="385" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A385" s="1" t="s">
         <v>51</v>
       </c>
@@ -21895,7 +21905,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="386" spans="1:15" ht="15" customHeight="1">
+    <row r="386" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A386" s="1" t="s">
         <v>51</v>
       </c>
@@ -21942,7 +21952,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="387" spans="1:15" ht="15" customHeight="1">
+    <row r="387" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A387" s="1" t="s">
         <v>51</v>
       </c>
@@ -21989,7 +21999,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="388" spans="1:15" ht="15" customHeight="1">
+    <row r="388" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A388" s="1" t="s">
         <v>51</v>
       </c>
@@ -22036,7 +22046,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="389" spans="1:15" ht="15" customHeight="1">
+    <row r="389" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A389" s="1" t="s">
         <v>51</v>
       </c>
@@ -22083,7 +22093,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="390" spans="1:15" ht="15" customHeight="1">
+    <row r="390" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A390" s="1" t="s">
         <v>51</v>
       </c>
@@ -22130,7 +22140,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="391" spans="1:15" ht="15" customHeight="1">
+    <row r="391" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A391" s="1" t="s">
         <v>51</v>
       </c>
@@ -22177,7 +22187,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="392" spans="1:15" ht="15" customHeight="1">
+    <row r="392" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A392" s="1" t="s">
         <v>51</v>
       </c>
@@ -22224,7 +22234,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="393" spans="1:15" ht="15" customHeight="1">
+    <row r="393" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A393" s="1" t="s">
         <v>51</v>
       </c>
@@ -22271,7 +22281,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="394" spans="1:15" ht="15" customHeight="1">
+    <row r="394" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A394" s="1" t="s">
         <v>51</v>
       </c>
@@ -22318,7 +22328,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="395" spans="1:15" ht="15" customHeight="1">
+    <row r="395" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A395" s="1" t="s">
         <v>51</v>
       </c>
@@ -22365,7 +22375,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="396" spans="1:15" ht="15" customHeight="1">
+    <row r="396" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A396" s="1" t="s">
         <v>51</v>
       </c>
@@ -22412,7 +22422,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="397" spans="1:15" ht="15" customHeight="1">
+    <row r="397" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A397" s="1" t="s">
         <v>51</v>
       </c>
@@ -22459,7 +22469,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="398" spans="1:15" ht="15" customHeight="1">
+    <row r="398" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A398" s="1" t="s">
         <v>51</v>
       </c>
@@ -22506,7 +22516,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="399" spans="1:15" ht="15" customHeight="1">
+    <row r="399" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A399" s="1" t="s">
         <v>51</v>
       </c>
@@ -22553,7 +22563,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="400" spans="1:15" ht="15" customHeight="1">
+    <row r="400" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A400" s="1" t="s">
         <v>51</v>
       </c>
@@ -22600,7 +22610,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="401" spans="1:15" ht="15" customHeight="1">
+    <row r="401" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A401" s="1" t="s">
         <v>51</v>
       </c>
@@ -22647,7 +22657,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="402" spans="1:15" ht="15" customHeight="1">
+    <row r="402" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A402" s="1" t="s">
         <v>51</v>
       </c>
@@ -22694,7 +22704,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="403" spans="1:15" ht="15" customHeight="1">
+    <row r="403" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A403" s="1" t="s">
         <v>51</v>
       </c>
@@ -22741,7 +22751,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="404" spans="1:15" ht="15" customHeight="1">
+    <row r="404" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A404" s="1" t="s">
         <v>51</v>
       </c>
@@ -22788,7 +22798,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="405" spans="1:15" ht="15" customHeight="1">
+    <row r="405" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A405" s="1" t="s">
         <v>0</v>
       </c>
@@ -22835,7 +22845,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="406" spans="1:15" ht="15" customHeight="1">
+    <row r="406" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A406" s="1" t="s">
         <v>0</v>
       </c>
@@ -22882,7 +22892,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="407" spans="1:15" ht="15" customHeight="1">
+    <row r="407" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A407" s="1" t="s">
         <v>0</v>
       </c>
@@ -22929,7 +22939,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="408" spans="1:15" ht="15" customHeight="1">
+    <row r="408" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A408" s="1" t="s">
         <v>0</v>
       </c>
@@ -22976,7 +22986,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="409" spans="1:15" ht="15" customHeight="1">
+    <row r="409" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A409" s="1" t="s">
         <v>0</v>
       </c>
@@ -23023,7 +23033,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="410" spans="1:15" ht="15" customHeight="1">
+    <row r="410" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A410" s="1" t="s">
         <v>0</v>
       </c>
@@ -23070,7 +23080,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="411" spans="1:15" ht="15" customHeight="1">
+    <row r="411" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A411" s="1" t="s">
         <v>0</v>
       </c>
@@ -23117,7 +23127,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="412" spans="1:15" ht="15" customHeight="1">
+    <row r="412" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A412" s="1" t="s">
         <v>0</v>
       </c>
@@ -23164,7 +23174,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="413" spans="1:15" ht="15" customHeight="1">
+    <row r="413" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A413" s="1" t="s">
         <v>0</v>
       </c>
@@ -23211,7 +23221,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="414" spans="1:15" ht="15" customHeight="1">
+    <row r="414" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A414" s="1" t="s">
         <v>0</v>
       </c>
@@ -23258,7 +23268,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="415" spans="1:15" ht="15" customHeight="1">
+    <row r="415" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A415" s="1" t="s">
         <v>0</v>
       </c>
@@ -23305,7 +23315,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="416" spans="1:15" ht="15" customHeight="1">
+    <row r="416" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A416" s="1" t="s">
         <v>0</v>
       </c>
@@ -23352,7 +23362,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="417" spans="1:15" ht="15" customHeight="1">
+    <row r="417" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A417" s="1" t="s">
         <v>0</v>
       </c>
@@ -23399,7 +23409,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="418" spans="1:15" ht="15" customHeight="1">
+    <row r="418" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A418" s="1" t="s">
         <v>0</v>
       </c>
@@ -23446,7 +23456,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="419" spans="1:15" ht="15" customHeight="1">
+    <row r="419" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A419" s="1" t="s">
         <v>0</v>
       </c>
@@ -23493,7 +23503,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="420" spans="1:15" ht="15" customHeight="1">
+    <row r="420" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A420" s="1" t="s">
         <v>0</v>
       </c>
@@ -23540,7 +23550,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="421" spans="1:15" ht="15" customHeight="1">
+    <row r="421" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A421" s="1" t="s">
         <v>0</v>
       </c>
@@ -23587,7 +23597,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="422" spans="1:15" ht="15" customHeight="1">
+    <row r="422" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A422" s="1" t="s">
         <v>0</v>
       </c>
@@ -23634,7 +23644,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="423" spans="1:15" ht="15" customHeight="1">
+    <row r="423" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A423" s="1" t="s">
         <v>0</v>
       </c>
@@ -23681,7 +23691,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="424" spans="1:15" ht="15" customHeight="1">
+    <row r="424" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A424" s="1" t="s">
         <v>0</v>
       </c>
@@ -23728,7 +23738,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="425" spans="1:15" ht="15" customHeight="1">
+    <row r="425" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A425" s="1" t="s">
         <v>0</v>
       </c>
@@ -23775,7 +23785,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="426" spans="1:15" ht="15" customHeight="1">
+    <row r="426" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A426" s="1" t="s">
         <v>0</v>
       </c>
@@ -23822,7 +23832,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="427" spans="1:15" ht="15" customHeight="1">
+    <row r="427" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A427" s="1" t="s">
         <v>0</v>
       </c>
@@ -23869,7 +23879,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="428" spans="1:15" ht="15" customHeight="1">
+    <row r="428" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A428" s="1" t="s">
         <v>0</v>
       </c>
@@ -23916,7 +23926,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="429" spans="1:15" ht="15" customHeight="1">
+    <row r="429" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A429" s="1" t="s">
         <v>0</v>
       </c>
@@ -23963,7 +23973,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="430" spans="1:15" ht="15" customHeight="1">
+    <row r="430" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A430" s="1" t="s">
         <v>0</v>
       </c>
@@ -24010,7 +24020,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="431" spans="1:15" ht="15" customHeight="1">
+    <row r="431" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A431" s="1" t="s">
         <v>0</v>
       </c>
@@ -24057,7 +24067,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="432" spans="1:15" ht="15" customHeight="1">
+    <row r="432" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A432" s="1" t="s">
         <v>0</v>
       </c>
@@ -24104,7 +24114,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="433" spans="1:15" ht="15" customHeight="1">
+    <row r="433" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A433" s="1" t="s">
         <v>0</v>
       </c>
@@ -24151,7 +24161,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="434" spans="1:15" ht="15" customHeight="1">
+    <row r="434" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A434" s="1" t="s">
         <v>0</v>
       </c>
@@ -24198,7 +24208,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="435" spans="1:15" ht="15" customHeight="1">
+    <row r="435" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A435" s="1" t="s">
         <v>0</v>
       </c>
@@ -24245,7 +24255,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="436" spans="1:15" ht="15" customHeight="1">
+    <row r="436" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A436" s="1" t="s">
         <v>0</v>
       </c>
@@ -24292,7 +24302,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="437" spans="1:15" ht="15" customHeight="1">
+    <row r="437" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A437" s="1" t="s">
         <v>0</v>
       </c>
@@ -24339,7 +24349,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="438" spans="1:15" ht="15" customHeight="1">
+    <row r="438" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A438" s="1" t="s">
         <v>0</v>
       </c>
@@ -24386,7 +24396,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="439" spans="1:15" ht="15" customHeight="1">
+    <row r="439" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A439" s="1" t="s">
         <v>0</v>
       </c>
@@ -24433,7 +24443,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="440" spans="1:15" ht="15" customHeight="1">
+    <row r="440" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A440" s="1" t="s">
         <v>0</v>
       </c>
@@ -24480,7 +24490,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="441" spans="1:15" ht="15" customHeight="1">
+    <row r="441" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A441" s="1" t="s">
         <v>0</v>
       </c>
@@ -24527,7 +24537,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="442" spans="1:15" ht="15" customHeight="1">
+    <row r="442" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A442" s="1" t="s">
         <v>0</v>
       </c>
@@ -24574,7 +24584,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="443" spans="1:15" ht="15" customHeight="1">
+    <row r="443" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A443" s="1" t="s">
         <v>0</v>
       </c>
@@ -24621,7 +24631,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="444" spans="1:15" ht="15" customHeight="1">
+    <row r="444" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A444" s="1" t="s">
         <v>0</v>
       </c>
@@ -24668,7 +24678,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="445" spans="1:15" ht="15" customHeight="1">
+    <row r="445" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A445" s="1" t="s">
         <v>0</v>
       </c>
@@ -24715,7 +24725,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="446" spans="1:15" ht="15" customHeight="1">
+    <row r="446" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A446" s="1" t="s">
         <v>0</v>
       </c>
@@ -24762,7 +24772,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="447" spans="1:15" ht="15" customHeight="1">
+    <row r="447" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A447" s="1" t="s">
         <v>0</v>
       </c>
@@ -24809,7 +24819,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="448" spans="1:15" ht="15" customHeight="1">
+    <row r="448" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A448" s="1" t="s">
         <v>0</v>
       </c>
@@ -24856,7 +24866,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="449" spans="1:15" ht="15" customHeight="1">
+    <row r="449" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A449" s="1" t="s">
         <v>0</v>
       </c>
@@ -24903,7 +24913,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="450" spans="1:15" ht="15" customHeight="1">
+    <row r="450" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A450" s="1" t="s">
         <v>0</v>
       </c>
@@ -24950,7 +24960,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="451" spans="1:15" ht="15" customHeight="1">
+    <row r="451" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A451" s="1" t="s">
         <v>0</v>
       </c>
@@ -24997,7 +25007,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="452" spans="1:15" ht="15" customHeight="1">
+    <row r="452" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A452" s="1" t="s">
         <v>0</v>
       </c>
@@ -25044,7 +25054,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="453" spans="1:15" ht="15" customHeight="1">
+    <row r="453" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A453" s="1" t="s">
         <v>0</v>
       </c>
@@ -25091,7 +25101,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="454" spans="1:15" ht="15" customHeight="1">
+    <row r="454" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A454" s="1" t="s">
         <v>0</v>
       </c>
@@ -25138,7 +25148,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="455" spans="1:15" ht="15" customHeight="1">
+    <row r="455" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A455" s="1" t="s">
         <v>0</v>
       </c>
@@ -25185,7 +25195,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="456" spans="1:15" ht="15" customHeight="1">
+    <row r="456" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A456" s="1" t="s">
         <v>0</v>
       </c>
@@ -25232,7 +25242,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="457" spans="1:15" ht="15" customHeight="1">
+    <row r="457" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A457" s="1" t="s">
         <v>0</v>
       </c>
@@ -25279,7 +25289,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="458" spans="1:15" ht="15" customHeight="1">
+    <row r="458" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A458" s="1" t="s">
         <v>0</v>
       </c>
@@ -25326,7 +25336,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="459" spans="1:15" ht="15" customHeight="1">
+    <row r="459" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A459" s="1" t="s">
         <v>0</v>
       </c>
@@ -25373,7 +25383,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="460" spans="1:15" ht="15" customHeight="1">
+    <row r="460" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A460" s="1" t="s">
         <v>0</v>
       </c>
@@ -25420,7 +25430,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="461" spans="1:15" ht="15" customHeight="1">
+    <row r="461" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A461" s="1" t="s">
         <v>0</v>
       </c>
@@ -25467,7 +25477,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="462" spans="1:15" ht="15" customHeight="1">
+    <row r="462" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A462" s="1" t="s">
         <v>0</v>
       </c>
@@ -25514,7 +25524,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="463" spans="1:15" ht="15" customHeight="1">
+    <row r="463" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A463" s="1" t="s">
         <v>0</v>
       </c>
@@ -25561,7 +25571,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="464" spans="1:15" ht="15" customHeight="1">
+    <row r="464" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A464" s="1" t="s">
         <v>0</v>
       </c>
@@ -25608,7 +25618,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="465" spans="1:15" ht="15" customHeight="1">
+    <row r="465" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A465" s="1" t="s">
         <v>0</v>
       </c>
@@ -25655,12 +25665,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="466" spans="1:15" ht="15" customHeight="1">
+    <row r="466" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A466" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B466" t="s">
-        <v>1</v>
+        <v>1129</v>
       </c>
       <c r="C466" s="1" t="s">
         <v>1025</v>
@@ -25702,12 +25712,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="467" spans="1:15" ht="15" customHeight="1">
+    <row r="467" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A467" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B467" t="s">
-        <v>1</v>
+        <v>1129</v>
       </c>
       <c r="C467" s="1" t="s">
         <v>1017</v>
@@ -25749,12 +25759,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="468" spans="1:15" ht="15" customHeight="1">
+    <row r="468" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A468" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B468" t="s">
-        <v>1</v>
+        <v>1129</v>
       </c>
       <c r="C468" s="1" t="s">
         <v>1027</v>
@@ -25796,12 +25806,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="469" spans="1:15" ht="15" customHeight="1">
+    <row r="469" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A469" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B469" t="s">
-        <v>1</v>
+        <v>1129</v>
       </c>
       <c r="C469" s="1" t="s">
         <v>1028</v>
@@ -25843,12 +25853,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="470" spans="1:15" ht="15" customHeight="1">
+    <row r="470" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A470" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B470" t="s">
-        <v>1</v>
+        <v>1129</v>
       </c>
       <c r="C470" s="1" t="s">
         <v>1029</v>
@@ -25890,12 +25900,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="471" spans="1:15" ht="15" customHeight="1">
+    <row r="471" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A471" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B471" t="s">
-        <v>1</v>
+        <v>1129</v>
       </c>
       <c r="C471" s="1" t="s">
         <v>1030</v>
@@ -25937,12 +25947,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="472" spans="1:15" ht="15" customHeight="1">
+    <row r="472" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A472" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B472" t="s">
-        <v>1</v>
+        <v>1129</v>
       </c>
       <c r="C472" s="1" t="s">
         <v>1031</v>
@@ -25984,12 +25994,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="473" spans="1:15" ht="15" customHeight="1">
+    <row r="473" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A473" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B473" t="s">
-        <v>1</v>
+        <v>1129</v>
       </c>
       <c r="C473" s="1" t="s">
         <v>1032</v>
@@ -26031,12 +26041,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="474" spans="1:15" ht="15" customHeight="1">
+    <row r="474" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A474" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B474" t="s">
-        <v>1</v>
+        <v>1129</v>
       </c>
       <c r="C474" s="1" t="s">
         <v>1033</v>
@@ -26078,12 +26088,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="475" spans="1:15" ht="15" customHeight="1">
+    <row r="475" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A475" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B475" t="s">
-        <v>1</v>
+        <v>1129</v>
       </c>
       <c r="C475" s="1" t="s">
         <v>1034</v>
@@ -26125,12 +26135,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="476" spans="1:15" ht="15" customHeight="1">
+    <row r="476" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A476" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B476" t="s">
-        <v>1</v>
+        <v>1129</v>
       </c>
       <c r="C476" s="1" t="s">
         <v>1035</v>
@@ -26172,12 +26182,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="477" spans="1:15" ht="15" customHeight="1">
+    <row r="477" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A477" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B477" t="s">
-        <v>1</v>
+        <v>1129</v>
       </c>
       <c r="C477" s="1" t="s">
         <v>1036</v>
@@ -26219,12 +26229,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="478" spans="1:15" ht="15" customHeight="1">
+    <row r="478" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A478" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B478" t="s">
-        <v>1</v>
+        <v>1129</v>
       </c>
       <c r="C478" s="1" t="s">
         <v>1037</v>
@@ -26266,12 +26276,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="479" spans="1:15" ht="15" customHeight="1">
+    <row r="479" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A479" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B479" t="s">
-        <v>1</v>
+        <v>1129</v>
       </c>
       <c r="C479" s="1" t="s">
         <v>1038</v>

</xml_diff>

<commit_message>
updated SMDSDocument list for import
</commit_message>
<xml_diff>
--- a/SMDSDocuments.xlsx
+++ b/SMDSDocuments.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6720" uniqueCount="1133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6746" uniqueCount="1134">
   <si>
     <t>ULP</t>
   </si>
@@ -3418,6 +3418,9 @@
   </si>
   <si>
     <t>begin date, end date, EmployerType</t>
+  </si>
+  <si>
+    <t>MED Procedural Order</t>
   </si>
 </sst>
 </file>
@@ -3783,24 +3786,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O480"/>
+  <dimension ref="A1:O482"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="A63" sqref="A63"/>
+    <sheetView tabSelected="1" topLeftCell="D448" workbookViewId="0">
+      <selection activeCell="M470" sqref="M470"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="48.7109375" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.85546875" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="62.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="68.42578125" customWidth="1"/>
     <col min="5" max="5" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8" customWidth="1"/>
-    <col min="7" max="8" width="1.85546875" customWidth="1"/>
-    <col min="9" max="9" width="1.42578125" customWidth="1"/>
-    <col min="10" max="10" width="1.85546875" customWidth="1"/>
-    <col min="11" max="11" width="1.7109375" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" customWidth="1"/>
+    <col min="8" max="8" width="1.85546875" customWidth="1"/>
+    <col min="9" max="9" width="21" customWidth="1"/>
+    <col min="10" max="10" width="9" customWidth="1"/>
+    <col min="11" max="11" width="22.7109375" customWidth="1"/>
     <col min="12" max="12" width="6" customWidth="1"/>
     <col min="13" max="13" width="33.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.42578125" bestFit="1" customWidth="1"/>
@@ -25628,10 +25632,10 @@
         <v>182</v>
       </c>
       <c r="C465" s="1" t="s">
-        <v>294</v>
+        <v>1024</v>
       </c>
       <c r="D465" s="1" t="s">
-        <v>1050</v>
+        <v>1114</v>
       </c>
       <c r="E465">
         <v>1</v>
@@ -25646,7 +25650,7 @@
         <v>4</v>
       </c>
       <c r="I465" s="1" t="s">
-        <v>492</v>
+        <v>4</v>
       </c>
       <c r="J465" s="3" t="s">
         <v>4</v>
@@ -25675,10 +25679,10 @@
         <v>182</v>
       </c>
       <c r="C466" s="1" t="s">
-        <v>1024</v>
+        <v>1133</v>
       </c>
       <c r="D466" s="1" t="s">
-        <v>1114</v>
+        <v>491</v>
       </c>
       <c r="E466">
         <v>1</v>
@@ -25719,13 +25723,13 @@
         <v>0</v>
       </c>
       <c r="B467" t="s">
-        <v>1129</v>
+        <v>182</v>
       </c>
       <c r="C467" s="1" t="s">
-        <v>1025</v>
+        <v>202</v>
       </c>
       <c r="D467" s="1" t="s">
-        <v>1115</v>
+        <v>1039</v>
       </c>
       <c r="E467">
         <v>1</v>
@@ -25734,19 +25738,17 @@
         <v>4</v>
       </c>
       <c r="G467" s="1" t="s">
-        <v>1026</v>
+        <v>4</v>
       </c>
       <c r="H467" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I467" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="I467" s="1"/>
       <c r="J467" s="3" t="s">
-        <v>4</v>
+        <v>204</v>
       </c>
       <c r="K467" s="3" t="s">
-        <v>4</v>
+        <v>205</v>
       </c>
       <c r="L467" s="3" t="s">
         <v>4</v>
@@ -25766,13 +25768,13 @@
         <v>0</v>
       </c>
       <c r="B468" t="s">
-        <v>1129</v>
+        <v>182</v>
       </c>
       <c r="C468" s="1" t="s">
-        <v>1017</v>
+        <v>206</v>
       </c>
       <c r="D468" s="1" t="s">
-        <v>1116</v>
+        <v>1040</v>
       </c>
       <c r="E468">
         <v>1</v>
@@ -25781,19 +25783,17 @@
         <v>4</v>
       </c>
       <c r="G468" s="1" t="s">
-        <v>1026</v>
+        <v>4</v>
       </c>
       <c r="H468" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I468" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="I468" s="1"/>
       <c r="J468" s="3" t="s">
-        <v>4</v>
+        <v>208</v>
       </c>
       <c r="K468" s="3" t="s">
-        <v>4</v>
+        <v>205</v>
       </c>
       <c r="L468" s="3" t="s">
         <v>4</v>
@@ -25816,10 +25816,10 @@
         <v>1129</v>
       </c>
       <c r="C469" s="1" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
       <c r="D469" s="1" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
       <c r="E469">
         <v>1</v>
@@ -25863,10 +25863,10 @@
         <v>1129</v>
       </c>
       <c r="C470" s="1" t="s">
-        <v>1028</v>
+        <v>1017</v>
       </c>
       <c r="D470" s="1" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
       <c r="E470">
         <v>1</v>
@@ -25910,10 +25910,10 @@
         <v>1129</v>
       </c>
       <c r="C471" s="1" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
       <c r="D471" s="1" t="s">
-        <v>1119</v>
+        <v>1117</v>
       </c>
       <c r="E471">
         <v>1</v>
@@ -25957,10 +25957,10 @@
         <v>1129</v>
       </c>
       <c r="C472" s="1" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="D472" s="1" t="s">
-        <v>1120</v>
+        <v>1118</v>
       </c>
       <c r="E472">
         <v>1</v>
@@ -26004,10 +26004,10 @@
         <v>1129</v>
       </c>
       <c r="C473" s="1" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="D473" s="1" t="s">
-        <v>1121</v>
+        <v>1119</v>
       </c>
       <c r="E473">
         <v>1</v>
@@ -26051,10 +26051,10 @@
         <v>1129</v>
       </c>
       <c r="C474" s="1" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="D474" s="1" t="s">
-        <v>1122</v>
+        <v>1120</v>
       </c>
       <c r="E474">
         <v>1</v>
@@ -26098,10 +26098,10 @@
         <v>1129</v>
       </c>
       <c r="C475" s="1" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="D475" s="1" t="s">
-        <v>1123</v>
+        <v>1121</v>
       </c>
       <c r="E475">
         <v>1</v>
@@ -26145,10 +26145,10 @@
         <v>1129</v>
       </c>
       <c r="C476" s="1" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="D476" s="1" t="s">
-        <v>1124</v>
+        <v>1122</v>
       </c>
       <c r="E476">
         <v>1</v>
@@ -26192,10 +26192,10 @@
         <v>1129</v>
       </c>
       <c r="C477" s="1" t="s">
-        <v>1035</v>
+        <v>1033</v>
       </c>
       <c r="D477" s="1" t="s">
-        <v>1125</v>
+        <v>1123</v>
       </c>
       <c r="E477">
         <v>1</v>
@@ -26239,10 +26239,10 @@
         <v>1129</v>
       </c>
       <c r="C478" s="1" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
       <c r="D478" s="1" t="s">
-        <v>1126</v>
+        <v>1124</v>
       </c>
       <c r="E478">
         <v>1</v>
@@ -26286,10 +26286,10 @@
         <v>1129</v>
       </c>
       <c r="C479" s="1" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
       <c r="D479" s="1" t="s">
-        <v>1127</v>
+        <v>1125</v>
       </c>
       <c r="E479">
         <v>1</v>
@@ -26333,10 +26333,10 @@
         <v>1129</v>
       </c>
       <c r="C480" s="1" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="D480" s="1" t="s">
-        <v>1128</v>
+        <v>1126</v>
       </c>
       <c r="E480">
         <v>1</v>
@@ -26369,6 +26369,100 @@
         <v>4</v>
       </c>
       <c r="O480" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="481" spans="1:15" ht="15" customHeight="1">
+      <c r="A481" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B481" t="s">
+        <v>1129</v>
+      </c>
+      <c r="C481" s="1" t="s">
+        <v>1037</v>
+      </c>
+      <c r="D481" s="1" t="s">
+        <v>1127</v>
+      </c>
+      <c r="E481">
+        <v>1</v>
+      </c>
+      <c r="F481" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G481" s="1" t="s">
+        <v>1026</v>
+      </c>
+      <c r="H481" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I481" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J481" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K481" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="L481" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="M481" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="N481" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="O481" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="482" spans="1:15" ht="15" customHeight="1">
+      <c r="A482" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B482" t="s">
+        <v>1129</v>
+      </c>
+      <c r="C482" s="1" t="s">
+        <v>1038</v>
+      </c>
+      <c r="D482" s="1" t="s">
+        <v>1128</v>
+      </c>
+      <c r="E482">
+        <v>1</v>
+      </c>
+      <c r="F482" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G482" s="1" t="s">
+        <v>1026</v>
+      </c>
+      <c r="H482" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I482" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J482" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K482" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="L482" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="M482" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="N482" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="O482" s="3" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>